<commit_message>
FordAuto: Added Used Vehicle and Vehicle Purchase Info Classes
</commit_message>
<xml_diff>
--- a/CoOpsAuto/src/test/resources/TestData/Ford_UI_QA_TestData.xlsx
+++ b/CoOpsAuto/src/test/resources/TestData/Ford_UI_QA_TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>TestName</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>James Miteshtest</t>
+  </si>
+  <si>
+    <t>validate_Ford_E2EScenario_2Driver_2Vehicle</t>
   </si>
 </sst>
 </file>
@@ -631,10 +634,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,9 +753,57 @@
         <v>28</v>
       </c>
     </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="4">
+        <v>20</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>